<commit_message>
atualizacao matriz de risco
</commit_message>
<xml_diff>
--- a/database/pasta_pdf/TabelaAtual.xlsx
+++ b/database/pasta_pdf/TabelaAtual.xlsx
@@ -1390,40 +1390,40 @@
     <t>MANOEL FEITOSA LIMA</t>
   </si>
   <si>
-    <t>785810/2024-163/00</t>
-  </si>
-  <si>
-    <t>785810/2024-164/00</t>
-  </si>
-  <si>
-    <t>785810/2024-165/00</t>
-  </si>
-  <si>
-    <t>785810/2024-166/00</t>
-  </si>
-  <si>
-    <t>785810/2024-167/00</t>
-  </si>
-  <si>
-    <t>785810/2024-168/00</t>
-  </si>
-  <si>
-    <t>785810/2024-169/00</t>
-  </si>
-  <si>
-    <t>785810/2024-170/00</t>
-  </si>
-  <si>
-    <t>785810/2024-171/00</t>
-  </si>
-  <si>
-    <t>785810/2024-172/00</t>
-  </si>
-  <si>
-    <t>785810/2024-173/00</t>
-  </si>
-  <si>
-    <t>785810/2024-174/00</t>
+    <t>785810/2024-055/00</t>
+  </si>
+  <si>
+    <t>785810/2024-056/00</t>
+  </si>
+  <si>
+    <t>785810/2024-057/00</t>
+  </si>
+  <si>
+    <t>785810/2024-058/00</t>
+  </si>
+  <si>
+    <t>785810/2024-059/00</t>
+  </si>
+  <si>
+    <t>785810/2024-060/00</t>
+  </si>
+  <si>
+    <t>785810/2024-061/00</t>
+  </si>
+  <si>
+    <t>785810/2024-062/00</t>
+  </si>
+  <si>
+    <t>785810/2024-063/00</t>
+  </si>
+  <si>
+    <t>785810/2024-064/00</t>
+  </si>
+  <si>
+    <t>785810/2024-065/00</t>
+  </si>
+  <si>
+    <t>785810/2024-066/00</t>
   </si>
 </sst>
 </file>

</xml_diff>